<commit_message>
Added a bunch of stuff
</commit_message>
<xml_diff>
--- a/Dev IV Solo Project Rubric.xlsx
+++ b/Dev IV Solo Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{725561CE-93F4-49D2-8057-422CA4D5CC62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CA6C119-E225-4E8E-B99F-23A4FF29AA41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="1815" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="106">
   <si>
     <t>Milestone I Points</t>
   </si>
@@ -338,6 +337,12 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -931,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,19 +1067,19 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92))</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G89) + SUMIF(C91:C92, "X",B91:B92) + SUMIF(D91:D92, "X",B91:B92) + SUMIF(E91:E92, "X",B91:B92)</f>
-        <v>20</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1090,11 +1095,15 @@
       <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>26</v>
@@ -1123,11 +1132,15 @@
       <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92)  &gt; 20, SUMIF(E4:E89,"=I",G4:G89) + SUMIF(C91:C92, "X",B91:B92) - 20,0)</f>
@@ -1135,7 +1148,7 @@
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=II",G4:G89) + SUMIF(D91:D92, "X",B91:B92) - 20,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J6" s="17">
         <f>IF(SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) &gt; 20, SUMIF(E4:E89,"=III",G4:G89) + SUMIF(E91:E92, "X",B91:B92) - 20,0)</f>
@@ -1160,11 +1173,15 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>22</v>
@@ -1191,11 +1208,15 @@
       <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 20, IF(K4+H4 &gt; 20, 20- H4, K4),0)</f>
@@ -1203,11 +1224,11 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 20, IF(H10+I4 &gt; 20, 20- I4, H10),0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 20, IF(I10+J4 &gt; 20, 20- J4, I10),0)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1225,11 +1246,15 @@
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>25</v>
@@ -1256,19 +1281,23 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 20 &gt; 0, K4+H4 - 20, 0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 20 &gt; 0, H10+I4 - 20, 0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 20 &gt; 0, I10+J4 - 20, 0)</f>
@@ -1290,11 +1319,15 @@
       <c r="D11" s="5">
         <v>2</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
+      <c r="E11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G11" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -1365,11 +1398,15 @@
       <c r="D14" s="5">
         <v>4</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G14" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1390,11 +1427,15 @@
       <c r="D15" s="5">
         <v>2</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
+      <c r="E15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G15" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1583,11 +1624,15 @@
       <c r="D24" s="5">
         <v>3</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G24" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1719,11 +1764,15 @@
       <c r="D30" s="5">
         <v>2</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G30" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -1955,11 +2004,15 @@
       <c r="D40" s="5">
         <v>3</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G40" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -2903,11 +2956,15 @@
       <c r="D82" s="5">
         <v>3</v>
       </c>
-      <c r="E82" s="2"/>
-      <c r="F82" s="3"/>
+      <c r="E82" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G82" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
@@ -3088,8 +3145,12 @@
       <c r="C91" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D91" s="3"/>
-      <c r="E91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
@@ -3108,8 +3169,12 @@
       <c r="C92" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D92" s="3"/>
-      <c r="E92" s="3"/>
+      <c r="D92" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
@@ -3242,7 +3307,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>